<commit_message>
Removed collected amount in remittance upload XL
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_remittances.xlsx
+++ b/public/sample_uploads/capital_remittances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F794279D-6435-4C61-A7DD-FC82576D95A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F73251A-2384-4936-982F-4D0E0188C0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Status</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Collected Amount *</t>
   </si>
   <si>
     <t>Capital Call *</t>
@@ -437,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -450,52 +447,48 @@
     <col min="3" max="3" width="18.6875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.375" customWidth="1"/>
-    <col min="7" max="7" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
       </c>
       <c r="D2">
         <v>12000</v>
@@ -506,28 +499,25 @@
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="s">
+        <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="J2">
+      <c r="I2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>30000</v>
@@ -538,28 +528,25 @@
       <c r="F3">
         <v>5</v>
       </c>
-      <c r="G3">
-        <v>30000</v>
+      <c r="G3" t="s">
+        <v>7</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3">
+      <c r="I3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>15000</v>
@@ -570,28 +557,25 @@
       <c r="F4">
         <v>5</v>
       </c>
-      <c r="G4">
-        <v>0</v>
+      <c r="G4" t="s">
+        <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="I4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>12000</v>
@@ -602,28 +586,25 @@
       <c r="F5">
         <v>5</v>
       </c>
-      <c r="G5">
-        <v>12000</v>
+      <c r="G5" t="s">
+        <v>7</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5">
         <v>9</v>
       </c>
-      <c r="J5">
-        <v>9</v>
-      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>13000</v>
@@ -634,16 +615,13 @@
       <c r="F6">
         <v>5</v>
       </c>
-      <c r="G6">
-        <v>13000</v>
+      <c r="G6" t="s">
+        <v>7</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
       </c>
-      <c r="I6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6">
+      <c r="I6">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added check to see that the docs and valuations can be ordered in the… (#722)
* Added check to see that the docs and valuations can be ordered in the partial

* Update remittances excel to not have data in the hidden column
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_remittances.xlsx
+++ b/public/sample_uploads/capital_remittances.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f10f76f200b1328/Desktop/Test/bulk files with notes/feb 25/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseem Karmali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{8B4A78C8-56D8-4099-B922-D68EEFB18F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F0BFA49-3396-4C7B-98D6-D798B5261B1F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5633B29F-059E-48D9-92AC-9D8B92F104DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -792,7 +792,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1048576"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -867,9 +867,6 @@
       <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="G2" s="2">
-        <v>1200000</v>
-      </c>
       <c r="K2" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>